<commit_message>
Se modifica el archivo de visualización: Importación del notebook de funciones + visualizaciones que estaban en el otro notebook    -  TP_WeatherAUS: Se eliminan las visualizaciones y se escriben 4 funciones: Geolocalizacion, eliminacion de nans, escalado y conversión de columna Date
</commit_message>
<xml_diff>
--- a/TP pre-procesamiento de columnas.xlsx
+++ b/TP pre-procesamiento de columnas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aulamultimedia\MEGA\Especializacion en Inteligencia Artificial UBA\Materias\Bimestre 2\Analisis de datos\TP\analisis_datos_TP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08165B5-FD9F-45BE-9A5C-24F92C0E9E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0854FA77-F5E3-4F52-A8FA-7ED7E859C334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="39">
   <si>
     <t>Columna</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>Normalizar</t>
+  </si>
+  <si>
+    <t>Preprocesamiento 3</t>
+  </si>
+  <si>
+    <t>Analizar outliers</t>
   </si>
 </sst>
 </file>
@@ -520,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,10 +538,11 @@
     <col min="2" max="2" width="11.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" style="3" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -551,8 +558,11 @@
       <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
@@ -565,11 +575,12 @@
       <c r="D2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -582,11 +593,12 @@
       <c r="D3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
@@ -600,10 +612,13 @@
         <v>32</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
@@ -617,10 +632,13 @@
         <v>32</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
@@ -634,10 +652,13 @@
         <v>32</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
@@ -651,8 +672,9 @@
         <v>31</v>
       </c>
       <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
@@ -666,8 +688,9 @@
         <v>31</v>
       </c>
       <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
@@ -680,11 +703,12 @@
       <c r="D9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>13</v>
       </c>
@@ -698,10 +722,13 @@
         <v>32</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>15</v>
       </c>
@@ -714,11 +741,12 @@
       <c r="D11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>16</v>
       </c>
@@ -731,11 +759,12 @@
       <c r="D12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>17</v>
       </c>
@@ -749,10 +778,13 @@
         <v>32</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>26</v>
       </c>
@@ -766,10 +798,13 @@
         <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>25</v>
       </c>
@@ -783,10 +818,13 @@
         <v>32</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>18</v>
       </c>
@@ -800,10 +838,13 @@
         <v>32</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>24</v>
       </c>
@@ -817,10 +858,13 @@
         <v>32</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>19</v>
       </c>
@@ -834,10 +878,13 @@
         <v>32</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>20</v>
       </c>
@@ -851,8 +898,9 @@
         <v>31</v>
       </c>
       <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>21</v>
       </c>
@@ -866,8 +914,9 @@
         <v>31</v>
       </c>
       <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>22</v>
       </c>
@@ -881,8 +930,9 @@
         <v>33</v>
       </c>
       <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>23</v>
       </c>
@@ -896,8 +946,9 @@
         <v>33</v>
       </c>
       <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>27</v>
       </c>
@@ -910,11 +961,12 @@
       <c r="D23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="4"/>
+      <c r="F23" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>35</v>
       </c>
@@ -927,32 +979,33 @@
       <c r="D24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="4"/>
+      <c r="F24" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>